<commit_message>
boton subir excel listo
</commit_message>
<xml_diff>
--- a/formato-postulante (1).xlsx
+++ b/formato-postulante (1).xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73ABA733-EB60-48E5-A5D1-5852DD3BD2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21012" windowHeight="6192"/>
   </bookViews>
   <sheets>
     <sheet name="Postulantes" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>OM</t>
   </si>
@@ -45,12 +44,72 @@
   </si>
   <si>
     <t>cant. Plazas</t>
+  </si>
+  <si>
+    <t>ASDasd</t>
+  </si>
+  <si>
+    <t>dassda</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>sadadsa</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>dsaads</t>
+  </si>
+  <si>
+    <t>sda</t>
+  </si>
+  <si>
+    <t>dsadas</t>
+  </si>
+  <si>
+    <t>dadsads</t>
+  </si>
+  <si>
+    <t>adsasd</t>
+  </si>
+  <si>
+    <t>adssda</t>
+  </si>
+  <si>
+    <t>CHOFER</t>
+  </si>
+  <si>
+    <t>GOF</t>
+  </si>
+  <si>
+    <t>CENATE</t>
+  </si>
+  <si>
+    <t>olivos</t>
+  </si>
+  <si>
+    <t>lince</t>
+  </si>
+  <si>
+    <t>smp</t>
+  </si>
+  <si>
+    <t>centro</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,26 +460,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,22 +493,177 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22B7A28-109B-4DF4-AE4D-30C50A14076C}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -461,6 +675,61 @@
       </c>
       <c r="D1" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>